<commit_message>
finished yoga paper again and resubmitted it online yay cross fingers toes and eyes
</commit_message>
<xml_diff>
--- a/p3_sec_outcomes_kyle.xlsx
+++ b/p3_sec_outcomes_kyle.xlsx
@@ -705,8 +705,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-543256832"/>
-        <c:axId val="-543257376"/>
+        <c:axId val="1480057312"/>
+        <c:axId val="1480066016"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -966,11 +966,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-543256832"/>
-        <c:axId val="-543257376"/>
+        <c:axId val="1480057312"/>
+        <c:axId val="1480066016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-543256832"/>
+        <c:axId val="1480057312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,7 +1012,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543257376"/>
+        <c:crossAx val="1480066016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1021,7 +1021,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-543257376"/>
+        <c:axId val="1480066016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1073,7 +1073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543256832"/>
+        <c:crossAx val="1480057312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1180,8 +1180,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-543255744"/>
-        <c:axId val="-543266080"/>
+        <c:axId val="1480068736"/>
+        <c:axId val="1480056224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1441,11 +1441,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-543255744"/>
-        <c:axId val="-543266080"/>
+        <c:axId val="1480068736"/>
+        <c:axId val="1480056224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-543255744"/>
+        <c:axId val="1480068736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1487,7 +1487,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543266080"/>
+        <c:crossAx val="1480056224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1496,7 +1496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-543266080"/>
+        <c:axId val="1480056224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="24"/>
@@ -1549,7 +1549,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543255744"/>
+        <c:crossAx val="1480068736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="6"/>
@@ -1657,8 +1657,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="500"/>
-        <c:axId val="-543264992"/>
-        <c:axId val="-543264448"/>
+        <c:axId val="1480066560"/>
+        <c:axId val="1480067648"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1918,11 +1918,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-543264992"/>
-        <c:axId val="-543264448"/>
+        <c:axId val="1480066560"/>
+        <c:axId val="1480067648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-543264992"/>
+        <c:axId val="1480066560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1964,7 +1964,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543264448"/>
+        <c:crossAx val="1480067648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1973,7 +1973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-543264448"/>
+        <c:axId val="1480067648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="28"/>
@@ -2026,7 +2026,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-543264992"/>
+        <c:crossAx val="1480066560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -5313,7 +5313,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+      <selection activeCell="T29" sqref="T29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6049,7 +6049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -6137,7 +6137,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -6268,8 +6268,12 @@
       <c r="Q21">
         <v>19</v>
       </c>
+      <c r="S21">
+        <f>AVERAGE(C2:C5)+AVERAGE(C15:C25)</f>
+        <v>113.11363636363637</v>
+      </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -6312,8 +6316,12 @@
       <c r="Q22">
         <v>20</v>
       </c>
+      <c r="S22">
+        <f>AVERAGE(C6:C14)+AVERAGE(C26:C34)</f>
+        <v>129.77777777777777</v>
+      </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -6356,8 +6364,16 @@
       <c r="Q23">
         <v>21</v>
       </c>
+      <c r="S23">
+        <f>S22-S21</f>
+        <v>16.664141414141397</v>
+      </c>
+      <c r="T23">
+        <f>_xlfn.STDEV.P(C2:C5, C15:C25)</f>
+        <v>25.242468623774144</v>
+      </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -6400,8 +6416,16 @@
       <c r="Q24">
         <v>22</v>
       </c>
+      <c r="S24">
+        <f>S23/T26</f>
+        <v>0.85916351711323047</v>
+      </c>
+      <c r="T24">
+        <f>_xlfn.STDEV.P(C6:C14, C26:C34)</f>
+        <v>10.733586378429619</v>
+      </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -6444,8 +6468,12 @@
       <c r="Q25">
         <v>23</v>
       </c>
+      <c r="T25">
+        <f>(POWER(T23, 2) + POWER(T24, 2))/2</f>
+        <v>376.19604938271596</v>
+      </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -6497,8 +6525,12 @@
       <c r="Q26">
         <v>24</v>
       </c>
+      <c r="T26">
+        <f>SQRT(T25)</f>
+        <v>19.395774008343054</v>
+      </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -6542,7 +6574,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>23</v>
       </c>
@@ -6586,7 +6618,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -6630,7 +6662,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>23</v>
       </c>
@@ -6674,7 +6706,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>23</v>
       </c>
@@ -6718,7 +6750,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>23</v>
       </c>

</xml_diff>